<commit_message>
Commit date: 10.04.2020. Code for ML with keras, tensorflow
</commit_message>
<xml_diff>
--- a/output_data/test_dataset.xlsx
+++ b/output_data/test_dataset.xlsx
@@ -65641,6 +65641,12 @@
       <c r="G1305">
         <v>4</v>
       </c>
+      <c r="H1305">
+        <v>999</v>
+      </c>
+      <c r="I1305">
+        <v>999</v>
+      </c>
       <c r="J1305">
         <v>40000</v>
       </c>
@@ -65685,6 +65691,12 @@
       <c r="G1306">
         <v>1</v>
       </c>
+      <c r="H1306">
+        <v>999</v>
+      </c>
+      <c r="I1306">
+        <v>999</v>
+      </c>
       <c r="J1306">
         <v>10000</v>
       </c>
@@ -65729,6 +65741,12 @@
       <c r="G1307">
         <v>3</v>
       </c>
+      <c r="H1307">
+        <v>999</v>
+      </c>
+      <c r="I1307">
+        <v>999</v>
+      </c>
       <c r="J1307">
         <v>14000</v>
       </c>
@@ -65773,6 +65791,12 @@
       <c r="G1308">
         <v>3</v>
       </c>
+      <c r="H1308">
+        <v>999</v>
+      </c>
+      <c r="I1308">
+        <v>999</v>
+      </c>
       <c r="J1308">
         <v>19000</v>
       </c>
@@ -65817,6 +65841,12 @@
       <c r="G1309">
         <v>1</v>
       </c>
+      <c r="H1309">
+        <v>999</v>
+      </c>
+      <c r="I1309">
+        <v>999</v>
+      </c>
       <c r="J1309">
         <v>14000</v>
       </c>
@@ -65861,6 +65891,12 @@
       <c r="G1310">
         <v>3</v>
       </c>
+      <c r="H1310">
+        <v>999</v>
+      </c>
+      <c r="I1310">
+        <v>999</v>
+      </c>
       <c r="J1310">
         <v>10000</v>
       </c>
@@ -65905,6 +65941,12 @@
       <c r="G1311">
         <v>4</v>
       </c>
+      <c r="H1311">
+        <v>999</v>
+      </c>
+      <c r="I1311">
+        <v>999</v>
+      </c>
       <c r="J1311">
         <v>12000</v>
       </c>
@@ -65949,6 +65991,12 @@
       <c r="G1312">
         <v>4</v>
       </c>
+      <c r="H1312">
+        <v>999</v>
+      </c>
+      <c r="I1312">
+        <v>999</v>
+      </c>
       <c r="J1312">
         <v>30000</v>
       </c>
@@ -65993,6 +66041,12 @@
       <c r="G1313">
         <v>3</v>
       </c>
+      <c r="H1313">
+        <v>999</v>
+      </c>
+      <c r="I1313">
+        <v>999</v>
+      </c>
       <c r="J1313">
         <v>16000</v>
       </c>
@@ -66037,6 +66091,12 @@
       <c r="G1314">
         <v>3</v>
       </c>
+      <c r="H1314">
+        <v>999</v>
+      </c>
+      <c r="I1314">
+        <v>999</v>
+      </c>
       <c r="J1314">
         <v>6000</v>
       </c>
@@ -66081,6 +66141,12 @@
       <c r="G1315">
         <v>1</v>
       </c>
+      <c r="H1315">
+        <v>999</v>
+      </c>
+      <c r="I1315">
+        <v>999</v>
+      </c>
       <c r="J1315">
         <v>8200</v>
       </c>
@@ -66125,6 +66191,12 @@
       <c r="G1316">
         <v>3</v>
       </c>
+      <c r="H1316">
+        <v>999</v>
+      </c>
+      <c r="I1316">
+        <v>999</v>
+      </c>
       <c r="J1316">
         <v>23000</v>
       </c>
@@ -66169,6 +66241,12 @@
       <c r="G1317">
         <v>3</v>
       </c>
+      <c r="H1317">
+        <v>999</v>
+      </c>
+      <c r="I1317">
+        <v>999</v>
+      </c>
       <c r="J1317">
         <v>10000</v>
       </c>
@@ -66213,6 +66291,12 @@
       <c r="G1318">
         <v>4</v>
       </c>
+      <c r="H1318">
+        <v>999</v>
+      </c>
+      <c r="I1318">
+        <v>999</v>
+      </c>
       <c r="J1318">
         <v>11000</v>
       </c>
@@ -66257,6 +66341,12 @@
       <c r="G1319">
         <v>3</v>
       </c>
+      <c r="H1319">
+        <v>999</v>
+      </c>
+      <c r="I1319">
+        <v>999</v>
+      </c>
       <c r="J1319">
         <v>8000</v>
       </c>
@@ -66301,6 +66391,12 @@
       <c r="G1320">
         <v>1</v>
       </c>
+      <c r="H1320">
+        <v>999</v>
+      </c>
+      <c r="I1320">
+        <v>999</v>
+      </c>
       <c r="J1320">
         <v>40000</v>
       </c>
@@ -66345,6 +66441,12 @@
       <c r="G1321">
         <v>4</v>
       </c>
+      <c r="H1321">
+        <v>999</v>
+      </c>
+      <c r="I1321">
+        <v>999</v>
+      </c>
       <c r="J1321">
         <v>50000</v>
       </c>
@@ -66389,6 +66491,12 @@
       <c r="G1322">
         <v>1</v>
       </c>
+      <c r="H1322">
+        <v>999</v>
+      </c>
+      <c r="I1322">
+        <v>999</v>
+      </c>
       <c r="J1322">
         <v>8500</v>
       </c>
@@ -66433,6 +66541,12 @@
       <c r="G1323">
         <v>4</v>
       </c>
+      <c r="H1323">
+        <v>999</v>
+      </c>
+      <c r="I1323">
+        <v>999</v>
+      </c>
       <c r="J1323">
         <v>10200</v>
       </c>
@@ -66477,6 +66591,12 @@
       <c r="G1324">
         <v>4</v>
       </c>
+      <c r="H1324">
+        <v>999</v>
+      </c>
+      <c r="I1324">
+        <v>999</v>
+      </c>
       <c r="J1324">
         <v>40000</v>
       </c>
@@ -66521,6 +66641,12 @@
       <c r="G1325">
         <v>4</v>
       </c>
+      <c r="H1325">
+        <v>999</v>
+      </c>
+      <c r="I1325">
+        <v>999</v>
+      </c>
       <c r="J1325">
         <v>45000</v>
       </c>
@@ -66565,6 +66691,12 @@
       <c r="G1326">
         <v>4</v>
       </c>
+      <c r="H1326">
+        <v>999</v>
+      </c>
+      <c r="I1326">
+        <v>999</v>
+      </c>
       <c r="J1326">
         <v>8450</v>
       </c>
@@ -66609,6 +66741,12 @@
       <c r="G1327">
         <v>3</v>
       </c>
+      <c r="H1327">
+        <v>999</v>
+      </c>
+      <c r="I1327">
+        <v>999</v>
+      </c>
       <c r="J1327">
         <v>6500</v>
       </c>
@@ -66653,6 +66791,12 @@
       <c r="G1328">
         <v>4</v>
       </c>
+      <c r="H1328">
+        <v>999</v>
+      </c>
+      <c r="I1328">
+        <v>999</v>
+      </c>
       <c r="J1328">
         <v>10000</v>
       </c>
@@ -66697,6 +66841,12 @@
       <c r="G1329">
         <v>3</v>
       </c>
+      <c r="H1329">
+        <v>999</v>
+      </c>
+      <c r="I1329">
+        <v>999</v>
+      </c>
       <c r="J1329">
         <v>17000</v>
       </c>
@@ -66741,6 +66891,12 @@
       <c r="G1330">
         <v>4</v>
       </c>
+      <c r="H1330">
+        <v>999</v>
+      </c>
+      <c r="I1330">
+        <v>999</v>
+      </c>
       <c r="J1330">
         <v>13200</v>
       </c>
@@ -66785,6 +66941,12 @@
       <c r="G1331">
         <v>4</v>
       </c>
+      <c r="H1331">
+        <v>999</v>
+      </c>
+      <c r="I1331">
+        <v>999</v>
+      </c>
       <c r="J1331">
         <v>25000</v>
       </c>
@@ -66829,6 +66991,12 @@
       <c r="G1332">
         <v>4</v>
       </c>
+      <c r="H1332">
+        <v>999</v>
+      </c>
+      <c r="I1332">
+        <v>999</v>
+      </c>
       <c r="J1332">
         <v>10000</v>
       </c>
@@ -66873,6 +67041,12 @@
       <c r="G1333">
         <v>4</v>
       </c>
+      <c r="H1333">
+        <v>999</v>
+      </c>
+      <c r="I1333">
+        <v>999</v>
+      </c>
       <c r="J1333">
         <v>25000</v>
       </c>
@@ -66917,6 +67091,12 @@
       <c r="G1334">
         <v>3</v>
       </c>
+      <c r="H1334">
+        <v>999</v>
+      </c>
+      <c r="I1334">
+        <v>999</v>
+      </c>
       <c r="J1334">
         <v>18000</v>
       </c>
@@ -66961,6 +67141,12 @@
       <c r="G1335">
         <v>4</v>
       </c>
+      <c r="H1335">
+        <v>999</v>
+      </c>
+      <c r="I1335">
+        <v>999</v>
+      </c>
       <c r="J1335">
         <v>25000</v>
       </c>
@@ -67005,6 +67191,12 @@
       <c r="G1336">
         <v>1</v>
       </c>
+      <c r="H1336">
+        <v>999</v>
+      </c>
+      <c r="I1336">
+        <v>999</v>
+      </c>
       <c r="J1336">
         <v>120000</v>
       </c>
@@ -67049,6 +67241,12 @@
       <c r="G1337">
         <v>3</v>
       </c>
+      <c r="H1337">
+        <v>999</v>
+      </c>
+      <c r="I1337">
+        <v>999</v>
+      </c>
       <c r="J1337">
         <v>15000</v>
       </c>
@@ -67093,6 +67291,12 @@
       <c r="G1338">
         <v>4</v>
       </c>
+      <c r="H1338">
+        <v>999</v>
+      </c>
+      <c r="I1338">
+        <v>999</v>
+      </c>
       <c r="J1338">
         <v>20000</v>
       </c>
@@ -67137,6 +67341,12 @@
       <c r="G1339">
         <v>3</v>
       </c>
+      <c r="H1339">
+        <v>999</v>
+      </c>
+      <c r="I1339">
+        <v>999</v>
+      </c>
       <c r="J1339">
         <v>30000</v>
       </c>
@@ -67181,6 +67391,12 @@
       <c r="G1340">
         <v>3</v>
       </c>
+      <c r="H1340">
+        <v>999</v>
+      </c>
+      <c r="I1340">
+        <v>999</v>
+      </c>
       <c r="J1340">
         <v>4000</v>
       </c>
@@ -67225,6 +67441,12 @@
       <c r="G1341">
         <v>3</v>
       </c>
+      <c r="H1341">
+        <v>999</v>
+      </c>
+      <c r="I1341">
+        <v>999</v>
+      </c>
       <c r="J1341">
         <v>9000</v>
       </c>
@@ -67269,6 +67491,12 @@
       <c r="G1342">
         <v>4</v>
       </c>
+      <c r="H1342">
+        <v>999</v>
+      </c>
+      <c r="I1342">
+        <v>999</v>
+      </c>
       <c r="J1342">
         <v>25000</v>
       </c>
@@ -67313,6 +67541,12 @@
       <c r="G1343">
         <v>1</v>
       </c>
+      <c r="H1343">
+        <v>999</v>
+      </c>
+      <c r="I1343">
+        <v>999</v>
+      </c>
       <c r="J1343">
         <v>11500</v>
       </c>
@@ -67357,6 +67591,12 @@
       <c r="G1344">
         <v>4</v>
       </c>
+      <c r="H1344">
+        <v>999</v>
+      </c>
+      <c r="I1344">
+        <v>999</v>
+      </c>
       <c r="J1344">
         <v>60000</v>
       </c>
@@ -67401,6 +67641,12 @@
       <c r="G1345">
         <v>3</v>
       </c>
+      <c r="H1345">
+        <v>999</v>
+      </c>
+      <c r="I1345">
+        <v>999</v>
+      </c>
       <c r="J1345">
         <v>35000</v>
       </c>
@@ -67445,6 +67691,12 @@
       <c r="G1346">
         <v>4</v>
       </c>
+      <c r="H1346">
+        <v>999</v>
+      </c>
+      <c r="I1346">
+        <v>999</v>
+      </c>
       <c r="J1346">
         <v>15000</v>
       </c>
@@ -67489,6 +67741,12 @@
       <c r="G1347">
         <v>4</v>
       </c>
+      <c r="H1347">
+        <v>999</v>
+      </c>
+      <c r="I1347">
+        <v>999</v>
+      </c>
       <c r="J1347">
         <v>5000</v>
       </c>
@@ -67533,6 +67791,12 @@
       <c r="G1348">
         <v>3</v>
       </c>
+      <c r="H1348">
+        <v>999</v>
+      </c>
+      <c r="I1348">
+        <v>999</v>
+      </c>
       <c r="J1348">
         <v>12000</v>
       </c>
@@ -67577,6 +67841,12 @@
       <c r="G1349">
         <v>3</v>
       </c>
+      <c r="H1349">
+        <v>999</v>
+      </c>
+      <c r="I1349">
+        <v>999</v>
+      </c>
       <c r="J1349">
         <v>15000</v>
       </c>
@@ -67621,6 +67891,12 @@
       <c r="G1350">
         <v>3</v>
       </c>
+      <c r="H1350">
+        <v>999</v>
+      </c>
+      <c r="I1350">
+        <v>999</v>
+      </c>
       <c r="J1350">
         <v>15000</v>
       </c>
@@ -67665,6 +67941,12 @@
       <c r="G1351">
         <v>4</v>
       </c>
+      <c r="H1351">
+        <v>999</v>
+      </c>
+      <c r="I1351">
+        <v>999</v>
+      </c>
       <c r="J1351">
         <v>10000</v>
       </c>
@@ -67709,6 +67991,12 @@
       <c r="G1352">
         <v>4</v>
       </c>
+      <c r="H1352">
+        <v>999</v>
+      </c>
+      <c r="I1352">
+        <v>999</v>
+      </c>
       <c r="J1352">
         <v>12000</v>
       </c>
@@ -67753,6 +68041,12 @@
       <c r="G1353">
         <v>4</v>
       </c>
+      <c r="H1353">
+        <v>999</v>
+      </c>
+      <c r="I1353">
+        <v>999</v>
+      </c>
       <c r="J1353">
         <v>20000</v>
       </c>
@@ -67797,6 +68091,12 @@
       <c r="G1354">
         <v>2</v>
       </c>
+      <c r="H1354">
+        <v>999</v>
+      </c>
+      <c r="I1354">
+        <v>999</v>
+      </c>
       <c r="J1354">
         <v>12000</v>
       </c>
@@ -67841,6 +68141,12 @@
       <c r="G1355">
         <v>4</v>
       </c>
+      <c r="H1355">
+        <v>999</v>
+      </c>
+      <c r="I1355">
+        <v>999</v>
+      </c>
       <c r="J1355">
         <v>14000</v>
       </c>
@@ -67885,6 +68191,12 @@
       <c r="G1356">
         <v>3</v>
       </c>
+      <c r="H1356">
+        <v>999</v>
+      </c>
+      <c r="I1356">
+        <v>999</v>
+      </c>
       <c r="J1356">
         <v>10000</v>
       </c>
@@ -67929,6 +68241,12 @@
       <c r="G1357">
         <v>4</v>
       </c>
+      <c r="H1357">
+        <v>999</v>
+      </c>
+      <c r="I1357">
+        <v>999</v>
+      </c>
       <c r="J1357">
         <v>30000</v>
       </c>
@@ -67973,6 +68291,12 @@
       <c r="G1358">
         <v>3</v>
       </c>
+      <c r="H1358">
+        <v>999</v>
+      </c>
+      <c r="I1358">
+        <v>999</v>
+      </c>
       <c r="J1358">
         <v>12000</v>
       </c>
@@ -68017,6 +68341,12 @@
       <c r="G1359">
         <v>4</v>
       </c>
+      <c r="H1359">
+        <v>999</v>
+      </c>
+      <c r="I1359">
+        <v>999</v>
+      </c>
       <c r="J1359">
         <v>12000</v>
       </c>
@@ -68061,6 +68391,12 @@
       <c r="G1360">
         <v>3</v>
       </c>
+      <c r="H1360">
+        <v>999</v>
+      </c>
+      <c r="I1360">
+        <v>999</v>
+      </c>
       <c r="J1360">
         <v>50000</v>
       </c>
@@ -68105,6 +68441,12 @@
       <c r="G1361">
         <v>4</v>
       </c>
+      <c r="H1361">
+        <v>999</v>
+      </c>
+      <c r="I1361">
+        <v>999</v>
+      </c>
       <c r="J1361">
         <v>20000</v>
       </c>
@@ -68149,6 +68491,12 @@
       <c r="G1362">
         <v>4</v>
       </c>
+      <c r="H1362">
+        <v>999</v>
+      </c>
+      <c r="I1362">
+        <v>999</v>
+      </c>
       <c r="J1362">
         <v>23000</v>
       </c>
@@ -68193,6 +68541,12 @@
       <c r="G1363">
         <v>1</v>
       </c>
+      <c r="H1363">
+        <v>999</v>
+      </c>
+      <c r="I1363">
+        <v>999</v>
+      </c>
       <c r="J1363">
         <v>25000</v>
       </c>
@@ -68237,6 +68591,12 @@
       <c r="G1364">
         <v>3</v>
       </c>
+      <c r="H1364">
+        <v>999</v>
+      </c>
+      <c r="I1364">
+        <v>999</v>
+      </c>
       <c r="J1364">
         <v>12000</v>
       </c>
@@ -68281,6 +68641,12 @@
       <c r="G1365">
         <v>3</v>
       </c>
+      <c r="H1365">
+        <v>999</v>
+      </c>
+      <c r="I1365">
+        <v>999</v>
+      </c>
       <c r="J1365">
         <v>13000</v>
       </c>
@@ -68325,6 +68691,12 @@
       <c r="G1366">
         <v>3</v>
       </c>
+      <c r="H1366">
+        <v>999</v>
+      </c>
+      <c r="I1366">
+        <v>999</v>
+      </c>
       <c r="J1366">
         <v>9000</v>
       </c>
@@ -68369,6 +68741,12 @@
       <c r="G1367">
         <v>4</v>
       </c>
+      <c r="H1367">
+        <v>999</v>
+      </c>
+      <c r="I1367">
+        <v>999</v>
+      </c>
       <c r="J1367">
         <v>90000</v>
       </c>
@@ -68413,6 +68791,12 @@
       <c r="G1368">
         <v>3</v>
       </c>
+      <c r="H1368">
+        <v>999</v>
+      </c>
+      <c r="I1368">
+        <v>999</v>
+      </c>
       <c r="J1368">
         <v>10000</v>
       </c>
@@ -68457,6 +68841,12 @@
       <c r="G1369">
         <v>3</v>
       </c>
+      <c r="H1369">
+        <v>999</v>
+      </c>
+      <c r="I1369">
+        <v>999</v>
+      </c>
       <c r="J1369">
         <v>30000</v>
       </c>
@@ -68501,6 +68891,12 @@
       <c r="G1370">
         <v>4</v>
       </c>
+      <c r="H1370">
+        <v>999</v>
+      </c>
+      <c r="I1370">
+        <v>999</v>
+      </c>
       <c r="J1370">
         <v>20000</v>
       </c>
@@ -68545,6 +68941,12 @@
       <c r="G1371">
         <v>3</v>
       </c>
+      <c r="H1371">
+        <v>999</v>
+      </c>
+      <c r="I1371">
+        <v>999</v>
+      </c>
       <c r="J1371">
         <v>15000</v>
       </c>
@@ -68589,6 +68991,12 @@
       <c r="G1372">
         <v>4</v>
       </c>
+      <c r="H1372">
+        <v>999</v>
+      </c>
+      <c r="I1372">
+        <v>999</v>
+      </c>
       <c r="J1372">
         <v>12600</v>
       </c>
@@ -68633,6 +69041,12 @@
       <c r="G1373">
         <v>2</v>
       </c>
+      <c r="H1373">
+        <v>999</v>
+      </c>
+      <c r="I1373">
+        <v>999</v>
+      </c>
       <c r="J1373">
         <v>11000</v>
       </c>
@@ -68677,6 +69091,12 @@
       <c r="G1374">
         <v>3</v>
       </c>
+      <c r="H1374">
+        <v>999</v>
+      </c>
+      <c r="I1374">
+        <v>999</v>
+      </c>
       <c r="J1374">
         <v>23000</v>
       </c>
@@ -68721,6 +69141,12 @@
       <c r="G1375">
         <v>3</v>
       </c>
+      <c r="H1375">
+        <v>999</v>
+      </c>
+      <c r="I1375">
+        <v>999</v>
+      </c>
       <c r="J1375">
         <v>60000</v>
       </c>
@@ -68765,6 +69191,12 @@
       <c r="G1376">
         <v>3</v>
       </c>
+      <c r="H1376">
+        <v>999</v>
+      </c>
+      <c r="I1376">
+        <v>999</v>
+      </c>
       <c r="J1376">
         <v>15000</v>
       </c>
@@ -68809,6 +69241,12 @@
       <c r="G1377">
         <v>1</v>
       </c>
+      <c r="H1377">
+        <v>999</v>
+      </c>
+      <c r="I1377">
+        <v>999</v>
+      </c>
       <c r="J1377">
         <v>10000</v>
       </c>
@@ -68853,6 +69291,12 @@
       <c r="G1378">
         <v>4</v>
       </c>
+      <c r="H1378">
+        <v>999</v>
+      </c>
+      <c r="I1378">
+        <v>999</v>
+      </c>
       <c r="J1378">
         <v>20000</v>
       </c>
@@ -68897,6 +69341,12 @@
       <c r="G1379">
         <v>3</v>
       </c>
+      <c r="H1379">
+        <v>999</v>
+      </c>
+      <c r="I1379">
+        <v>999</v>
+      </c>
       <c r="J1379">
         <v>25000</v>
       </c>
@@ -68941,6 +69391,12 @@
       <c r="G1380">
         <v>4</v>
       </c>
+      <c r="H1380">
+        <v>999</v>
+      </c>
+      <c r="I1380">
+        <v>999</v>
+      </c>
       <c r="J1380">
         <v>6300</v>
       </c>
@@ -68985,6 +69441,12 @@
       <c r="G1381">
         <v>3</v>
       </c>
+      <c r="H1381">
+        <v>999</v>
+      </c>
+      <c r="I1381">
+        <v>999</v>
+      </c>
       <c r="J1381">
         <v>30000</v>
       </c>
@@ -69029,6 +69491,12 @@
       <c r="G1382">
         <v>4</v>
       </c>
+      <c r="H1382">
+        <v>999</v>
+      </c>
+      <c r="I1382">
+        <v>999</v>
+      </c>
       <c r="J1382">
         <v>90000</v>
       </c>
@@ -69073,6 +69541,12 @@
       <c r="G1383">
         <v>3</v>
       </c>
+      <c r="H1383">
+        <v>999</v>
+      </c>
+      <c r="I1383">
+        <v>999</v>
+      </c>
       <c r="J1383">
         <v>50000</v>
       </c>
@@ -69117,6 +69591,12 @@
       <c r="G1384">
         <v>4</v>
       </c>
+      <c r="H1384">
+        <v>999</v>
+      </c>
+      <c r="I1384">
+        <v>999</v>
+      </c>
       <c r="J1384">
         <v>40000</v>
       </c>
@@ -69161,6 +69641,12 @@
       <c r="G1385">
         <v>3</v>
       </c>
+      <c r="H1385">
+        <v>999</v>
+      </c>
+      <c r="I1385">
+        <v>999</v>
+      </c>
       <c r="J1385">
         <v>8500</v>
       </c>
@@ -69205,6 +69691,12 @@
       <c r="G1386">
         <v>5</v>
       </c>
+      <c r="H1386">
+        <v>999</v>
+      </c>
+      <c r="I1386">
+        <v>999</v>
+      </c>
       <c r="J1386">
         <v>50000</v>
       </c>
@@ -69249,6 +69741,12 @@
       <c r="G1387">
         <v>3</v>
       </c>
+      <c r="H1387">
+        <v>999</v>
+      </c>
+      <c r="I1387">
+        <v>999</v>
+      </c>
       <c r="J1387">
         <v>20000</v>
       </c>
@@ -69293,6 +69791,12 @@
       <c r="G1388">
         <v>1</v>
       </c>
+      <c r="H1388">
+        <v>999</v>
+      </c>
+      <c r="I1388">
+        <v>999</v>
+      </c>
       <c r="J1388">
         <v>15000</v>
       </c>
@@ -69337,6 +69841,12 @@
       <c r="G1389">
         <v>3</v>
       </c>
+      <c r="H1389">
+        <v>999</v>
+      </c>
+      <c r="I1389">
+        <v>999</v>
+      </c>
       <c r="J1389">
         <v>25000</v>
       </c>
@@ -69381,6 +69891,12 @@
       <c r="G1390">
         <v>3</v>
       </c>
+      <c r="H1390">
+        <v>999</v>
+      </c>
+      <c r="I1390">
+        <v>999</v>
+      </c>
       <c r="J1390">
         <v>9000</v>
       </c>
@@ -69425,6 +69941,12 @@
       <c r="G1391">
         <v>1</v>
       </c>
+      <c r="H1391">
+        <v>999</v>
+      </c>
+      <c r="I1391">
+        <v>999</v>
+      </c>
       <c r="J1391">
         <v>8000</v>
       </c>
@@ -69469,6 +69991,12 @@
       <c r="G1392">
         <v>3</v>
       </c>
+      <c r="H1392">
+        <v>999</v>
+      </c>
+      <c r="I1392">
+        <v>999</v>
+      </c>
       <c r="J1392">
         <v>10000</v>
       </c>
@@ -69513,6 +70041,12 @@
       <c r="G1393">
         <v>3</v>
       </c>
+      <c r="H1393">
+        <v>999</v>
+      </c>
+      <c r="I1393">
+        <v>999</v>
+      </c>
       <c r="J1393">
         <v>30000</v>
       </c>
@@ -69557,6 +70091,12 @@
       <c r="G1394">
         <v>1</v>
       </c>
+      <c r="H1394">
+        <v>999</v>
+      </c>
+      <c r="I1394">
+        <v>999</v>
+      </c>
       <c r="J1394">
         <v>35000</v>
       </c>
@@ -69601,6 +70141,12 @@
       <c r="G1395">
         <v>3</v>
       </c>
+      <c r="H1395">
+        <v>999</v>
+      </c>
+      <c r="I1395">
+        <v>999</v>
+      </c>
       <c r="J1395">
         <v>25000</v>
       </c>
@@ -69645,6 +70191,12 @@
       <c r="G1396">
         <v>3</v>
       </c>
+      <c r="H1396">
+        <v>999</v>
+      </c>
+      <c r="I1396">
+        <v>999</v>
+      </c>
       <c r="J1396">
         <v>12000</v>
       </c>
@@ -69689,6 +70241,12 @@
       <c r="G1397">
         <v>1</v>
       </c>
+      <c r="H1397">
+        <v>999</v>
+      </c>
+      <c r="I1397">
+        <v>999</v>
+      </c>
       <c r="J1397">
         <v>45000</v>
       </c>
@@ -69733,6 +70291,12 @@
       <c r="G1398">
         <v>3</v>
       </c>
+      <c r="H1398">
+        <v>999</v>
+      </c>
+      <c r="I1398">
+        <v>999</v>
+      </c>
       <c r="J1398">
         <v>20000</v>
       </c>
@@ -69777,6 +70341,12 @@
       <c r="G1399">
         <v>1</v>
       </c>
+      <c r="H1399">
+        <v>999</v>
+      </c>
+      <c r="I1399">
+        <v>999</v>
+      </c>
       <c r="J1399">
         <v>28000</v>
       </c>
@@ -69821,6 +70391,12 @@
       <c r="G1400">
         <v>4</v>
       </c>
+      <c r="H1400">
+        <v>999</v>
+      </c>
+      <c r="I1400">
+        <v>999</v>
+      </c>
       <c r="J1400">
         <v>3000</v>
       </c>
@@ -69865,6 +70441,12 @@
       <c r="G1401">
         <v>4</v>
       </c>
+      <c r="H1401">
+        <v>999</v>
+      </c>
+      <c r="I1401">
+        <v>999</v>
+      </c>
       <c r="J1401">
         <v>12000</v>
       </c>
@@ -69909,6 +70491,12 @@
       <c r="G1402">
         <v>1</v>
       </c>
+      <c r="H1402">
+        <v>999</v>
+      </c>
+      <c r="I1402">
+        <v>999</v>
+      </c>
       <c r="J1402">
         <v>25000</v>
       </c>
@@ -69953,6 +70541,12 @@
       <c r="G1403">
         <v>3</v>
       </c>
+      <c r="H1403">
+        <v>999</v>
+      </c>
+      <c r="I1403">
+        <v>999</v>
+      </c>
       <c r="J1403">
         <v>20000</v>
       </c>
@@ -69997,6 +70591,12 @@
       <c r="G1404">
         <v>1</v>
       </c>
+      <c r="H1404">
+        <v>999</v>
+      </c>
+      <c r="I1404">
+        <v>999</v>
+      </c>
       <c r="J1404">
         <v>50000</v>
       </c>
@@ -70041,6 +70641,12 @@
       <c r="G1405">
         <v>3</v>
       </c>
+      <c r="H1405">
+        <v>999</v>
+      </c>
+      <c r="I1405">
+        <v>999</v>
+      </c>
       <c r="J1405">
         <v>8400</v>
       </c>
@@ -70085,6 +70691,12 @@
       <c r="G1406">
         <v>1</v>
       </c>
+      <c r="H1406">
+        <v>999</v>
+      </c>
+      <c r="I1406">
+        <v>999</v>
+      </c>
       <c r="J1406">
         <v>15000</v>
       </c>
@@ -70129,6 +70741,12 @@
       <c r="G1407">
         <v>4</v>
       </c>
+      <c r="H1407">
+        <v>999</v>
+      </c>
+      <c r="I1407">
+        <v>999</v>
+      </c>
       <c r="J1407">
         <v>50000</v>
       </c>
@@ -70173,6 +70791,12 @@
       <c r="G1408">
         <v>4</v>
       </c>
+      <c r="H1408">
+        <v>999</v>
+      </c>
+      <c r="I1408">
+        <v>999</v>
+      </c>
       <c r="J1408">
         <v>60000</v>
       </c>
@@ -70217,6 +70841,12 @@
       <c r="G1409">
         <v>4</v>
       </c>
+      <c r="H1409">
+        <v>999</v>
+      </c>
+      <c r="I1409">
+        <v>999</v>
+      </c>
       <c r="J1409">
         <v>40000</v>
       </c>
@@ -70261,6 +70891,12 @@
       <c r="G1410">
         <v>1</v>
       </c>
+      <c r="H1410">
+        <v>999</v>
+      </c>
+      <c r="I1410">
+        <v>999</v>
+      </c>
       <c r="J1410">
         <v>45000</v>
       </c>
@@ -70305,6 +70941,12 @@
       <c r="G1411">
         <v>3</v>
       </c>
+      <c r="H1411">
+        <v>999</v>
+      </c>
+      <c r="I1411">
+        <v>999</v>
+      </c>
       <c r="J1411">
         <v>50000</v>
       </c>
@@ -70349,6 +70991,12 @@
       <c r="G1412">
         <v>3</v>
       </c>
+      <c r="H1412">
+        <v>999</v>
+      </c>
+      <c r="I1412">
+        <v>999</v>
+      </c>
       <c r="J1412">
         <v>12500</v>
       </c>
@@ -70393,6 +71041,12 @@
       <c r="G1413">
         <v>4</v>
       </c>
+      <c r="H1413">
+        <v>999</v>
+      </c>
+      <c r="I1413">
+        <v>999</v>
+      </c>
       <c r="J1413">
         <v>50000</v>
       </c>
@@ -70437,6 +71091,12 @@
       <c r="G1414">
         <v>1</v>
       </c>
+      <c r="H1414">
+        <v>999</v>
+      </c>
+      <c r="I1414">
+        <v>999</v>
+      </c>
       <c r="J1414">
         <v>8000</v>
       </c>
@@ -70481,6 +71141,12 @@
       <c r="G1415">
         <v>3</v>
       </c>
+      <c r="H1415">
+        <v>999</v>
+      </c>
+      <c r="I1415">
+        <v>999</v>
+      </c>
       <c r="J1415">
         <v>20000</v>
       </c>
@@ -70525,6 +71191,12 @@
       <c r="G1416">
         <v>1</v>
       </c>
+      <c r="H1416">
+        <v>999</v>
+      </c>
+      <c r="I1416">
+        <v>999</v>
+      </c>
       <c r="J1416">
         <v>8000</v>
       </c>
@@ -70569,6 +71241,12 @@
       <c r="G1417">
         <v>3</v>
       </c>
+      <c r="H1417">
+        <v>999</v>
+      </c>
+      <c r="I1417">
+        <v>999</v>
+      </c>
       <c r="J1417">
         <v>35000</v>
       </c>
@@ -70613,6 +71291,12 @@
       <c r="G1418">
         <v>3</v>
       </c>
+      <c r="H1418">
+        <v>999</v>
+      </c>
+      <c r="I1418">
+        <v>999</v>
+      </c>
       <c r="J1418">
         <v>15000</v>
       </c>
@@ -70657,6 +71341,12 @@
       <c r="G1419">
         <v>3</v>
       </c>
+      <c r="H1419">
+        <v>999</v>
+      </c>
+      <c r="I1419">
+        <v>999</v>
+      </c>
       <c r="J1419">
         <v>10000</v>
       </c>
@@ -70701,6 +71391,12 @@
       <c r="G1420">
         <v>4</v>
       </c>
+      <c r="H1420">
+        <v>999</v>
+      </c>
+      <c r="I1420">
+        <v>999</v>
+      </c>
       <c r="J1420">
         <v>11000</v>
       </c>
@@ -70745,6 +71441,12 @@
       <c r="G1421">
         <v>4</v>
       </c>
+      <c r="H1421">
+        <v>999</v>
+      </c>
+      <c r="I1421">
+        <v>999</v>
+      </c>
       <c r="J1421">
         <v>40000</v>
       </c>
@@ -70789,6 +71491,12 @@
       <c r="G1422">
         <v>3</v>
       </c>
+      <c r="H1422">
+        <v>999</v>
+      </c>
+      <c r="I1422">
+        <v>999</v>
+      </c>
       <c r="J1422">
         <v>20000</v>
       </c>
@@ -70833,6 +71541,12 @@
       <c r="G1423">
         <v>4</v>
       </c>
+      <c r="H1423">
+        <v>999</v>
+      </c>
+      <c r="I1423">
+        <v>999</v>
+      </c>
       <c r="J1423">
         <v>19000</v>
       </c>
@@ -70877,6 +71591,12 @@
       <c r="G1424">
         <v>4</v>
       </c>
+      <c r="H1424">
+        <v>999</v>
+      </c>
+      <c r="I1424">
+        <v>999</v>
+      </c>
       <c r="J1424">
         <v>15000</v>
       </c>
@@ -70921,6 +71641,12 @@
       <c r="G1425">
         <v>4</v>
       </c>
+      <c r="H1425">
+        <v>999</v>
+      </c>
+      <c r="I1425">
+        <v>999</v>
+      </c>
       <c r="J1425">
         <v>25000</v>
       </c>
@@ -70965,6 +71691,12 @@
       <c r="G1426">
         <v>4</v>
       </c>
+      <c r="H1426">
+        <v>999</v>
+      </c>
+      <c r="I1426">
+        <v>999</v>
+      </c>
       <c r="J1426">
         <v>58000</v>
       </c>
@@ -71009,6 +71741,12 @@
       <c r="G1427">
         <v>5</v>
       </c>
+      <c r="H1427">
+        <v>999</v>
+      </c>
+      <c r="I1427">
+        <v>999</v>
+      </c>
       <c r="J1427">
         <v>60000</v>
       </c>
@@ -71053,6 +71791,12 @@
       <c r="G1428">
         <v>3</v>
       </c>
+      <c r="H1428">
+        <v>999</v>
+      </c>
+      <c r="I1428">
+        <v>999</v>
+      </c>
       <c r="J1428">
         <v>15000</v>
       </c>
@@ -71097,6 +71841,12 @@
       <c r="G1429">
         <v>4</v>
       </c>
+      <c r="H1429">
+        <v>999</v>
+      </c>
+      <c r="I1429">
+        <v>999</v>
+      </c>
       <c r="J1429">
         <v>40000</v>
       </c>
@@ -71141,6 +71891,12 @@
       <c r="G1430">
         <v>4</v>
       </c>
+      <c r="H1430">
+        <v>999</v>
+      </c>
+      <c r="I1430">
+        <v>999</v>
+      </c>
       <c r="J1430">
         <v>5000</v>
       </c>
@@ -71185,6 +71941,12 @@
       <c r="G1431">
         <v>1</v>
       </c>
+      <c r="H1431">
+        <v>999</v>
+      </c>
+      <c r="I1431">
+        <v>999</v>
+      </c>
       <c r="J1431">
         <v>7700</v>
       </c>
@@ -71229,6 +71991,12 @@
       <c r="G1432">
         <v>3</v>
       </c>
+      <c r="H1432">
+        <v>999</v>
+      </c>
+      <c r="I1432">
+        <v>999</v>
+      </c>
       <c r="J1432">
         <v>8000</v>
       </c>
@@ -71273,6 +72041,12 @@
       <c r="G1433">
         <v>3</v>
       </c>
+      <c r="H1433">
+        <v>999</v>
+      </c>
+      <c r="I1433">
+        <v>999</v>
+      </c>
       <c r="J1433">
         <v>14000</v>
       </c>
@@ -71317,6 +72091,12 @@
       <c r="G1434">
         <v>1</v>
       </c>
+      <c r="H1434">
+        <v>999</v>
+      </c>
+      <c r="I1434">
+        <v>999</v>
+      </c>
       <c r="J1434">
         <v>30000</v>
       </c>
@@ -71361,6 +72141,12 @@
       <c r="G1435">
         <v>3</v>
       </c>
+      <c r="H1435">
+        <v>999</v>
+      </c>
+      <c r="I1435">
+        <v>999</v>
+      </c>
       <c r="J1435">
         <v>8000</v>
       </c>
@@ -71405,6 +72191,12 @@
       <c r="G1436">
         <v>2</v>
       </c>
+      <c r="H1436">
+        <v>999</v>
+      </c>
+      <c r="I1436">
+        <v>999</v>
+      </c>
       <c r="J1436">
         <v>30000</v>
       </c>
@@ -71449,6 +72241,12 @@
       <c r="G1437">
         <v>3</v>
       </c>
+      <c r="H1437">
+        <v>999</v>
+      </c>
+      <c r="I1437">
+        <v>999</v>
+      </c>
       <c r="J1437">
         <v>12000</v>
       </c>
@@ -71493,6 +72291,12 @@
       <c r="G1438">
         <v>3</v>
       </c>
+      <c r="H1438">
+        <v>999</v>
+      </c>
+      <c r="I1438">
+        <v>999</v>
+      </c>
       <c r="J1438">
         <v>25000</v>
       </c>
@@ -71537,6 +72341,12 @@
       <c r="G1439">
         <v>1</v>
       </c>
+      <c r="H1439">
+        <v>999</v>
+      </c>
+      <c r="I1439">
+        <v>999</v>
+      </c>
       <c r="J1439">
         <v>10000</v>
       </c>
@@ -71581,6 +72391,12 @@
       <c r="G1440">
         <v>4</v>
       </c>
+      <c r="H1440">
+        <v>999</v>
+      </c>
+      <c r="I1440">
+        <v>999</v>
+      </c>
       <c r="J1440">
         <v>35000</v>
       </c>
@@ -71625,6 +72441,12 @@
       <c r="G1441">
         <v>4</v>
       </c>
+      <c r="H1441">
+        <v>999</v>
+      </c>
+      <c r="I1441">
+        <v>999</v>
+      </c>
       <c r="J1441">
         <v>40000</v>
       </c>
@@ -71669,6 +72491,12 @@
       <c r="G1442">
         <v>4</v>
       </c>
+      <c r="H1442">
+        <v>999</v>
+      </c>
+      <c r="I1442">
+        <v>999</v>
+      </c>
       <c r="J1442">
         <v>50000</v>
       </c>
@@ -71713,6 +72541,12 @@
       <c r="G1443">
         <v>4</v>
       </c>
+      <c r="H1443">
+        <v>999</v>
+      </c>
+      <c r="I1443">
+        <v>999</v>
+      </c>
       <c r="J1443">
         <v>15000</v>
       </c>
@@ -71757,6 +72591,12 @@
       <c r="G1444">
         <v>4</v>
       </c>
+      <c r="H1444">
+        <v>999</v>
+      </c>
+      <c r="I1444">
+        <v>999</v>
+      </c>
       <c r="J1444">
         <v>12000</v>
       </c>
@@ -71801,6 +72641,12 @@
       <c r="G1445">
         <v>4</v>
       </c>
+      <c r="H1445">
+        <v>999</v>
+      </c>
+      <c r="I1445">
+        <v>999</v>
+      </c>
       <c r="J1445">
         <v>20000</v>
       </c>
@@ -71845,6 +72691,12 @@
       <c r="G1446">
         <v>4</v>
       </c>
+      <c r="H1446">
+        <v>999</v>
+      </c>
+      <c r="I1446">
+        <v>999</v>
+      </c>
       <c r="J1446">
         <v>12000</v>
       </c>
@@ -71889,6 +72741,12 @@
       <c r="G1447">
         <v>1</v>
       </c>
+      <c r="H1447">
+        <v>999</v>
+      </c>
+      <c r="I1447">
+        <v>999</v>
+      </c>
       <c r="J1447">
         <v>25000</v>
       </c>
@@ -71933,6 +72791,12 @@
       <c r="G1448">
         <v>1</v>
       </c>
+      <c r="H1448">
+        <v>999</v>
+      </c>
+      <c r="I1448">
+        <v>999</v>
+      </c>
       <c r="J1448">
         <v>20000</v>
       </c>
@@ -71977,6 +72841,12 @@
       <c r="G1449">
         <v>3</v>
       </c>
+      <c r="H1449">
+        <v>999</v>
+      </c>
+      <c r="I1449">
+        <v>999</v>
+      </c>
       <c r="J1449">
         <v>27000</v>
       </c>
@@ -72021,6 +72891,12 @@
       <c r="G1450">
         <v>2</v>
       </c>
+      <c r="H1450">
+        <v>999</v>
+      </c>
+      <c r="I1450">
+        <v>999</v>
+      </c>
       <c r="J1450">
         <v>20000</v>
       </c>
@@ -72065,6 +72941,12 @@
       <c r="G1451">
         <v>3</v>
       </c>
+      <c r="H1451">
+        <v>999</v>
+      </c>
+      <c r="I1451">
+        <v>999</v>
+      </c>
       <c r="J1451">
         <v>8900</v>
       </c>
@@ -72109,6 +72991,12 @@
       <c r="G1452">
         <v>3</v>
       </c>
+      <c r="H1452">
+        <v>999</v>
+      </c>
+      <c r="I1452">
+        <v>999</v>
+      </c>
       <c r="J1452">
         <v>30000</v>
       </c>
@@ -72153,6 +73041,12 @@
       <c r="G1453">
         <v>4</v>
       </c>
+      <c r="H1453">
+        <v>999</v>
+      </c>
+      <c r="I1453">
+        <v>999</v>
+      </c>
       <c r="J1453">
         <v>30000</v>
       </c>
@@ -72197,6 +73091,12 @@
       <c r="G1454">
         <v>4</v>
       </c>
+      <c r="H1454">
+        <v>999</v>
+      </c>
+      <c r="I1454">
+        <v>999</v>
+      </c>
       <c r="J1454">
         <v>30000</v>
       </c>
@@ -72241,6 +73141,12 @@
       <c r="G1455">
         <v>4</v>
       </c>
+      <c r="H1455">
+        <v>999</v>
+      </c>
+      <c r="I1455">
+        <v>999</v>
+      </c>
       <c r="J1455">
         <v>20000</v>
       </c>
@@ -72285,6 +73191,12 @@
       <c r="G1456">
         <v>1</v>
       </c>
+      <c r="H1456">
+        <v>999</v>
+      </c>
+      <c r="I1456">
+        <v>999</v>
+      </c>
       <c r="J1456">
         <v>22000</v>
       </c>
@@ -72329,6 +73241,12 @@
       <c r="G1457">
         <v>2</v>
       </c>
+      <c r="H1457">
+        <v>999</v>
+      </c>
+      <c r="I1457">
+        <v>999</v>
+      </c>
       <c r="J1457">
         <v>15000</v>
       </c>
@@ -72373,6 +73291,12 @@
       <c r="G1458">
         <v>4</v>
       </c>
+      <c r="H1458">
+        <v>999</v>
+      </c>
+      <c r="I1458">
+        <v>999</v>
+      </c>
       <c r="J1458">
         <v>10000</v>
       </c>
@@ -72417,6 +73341,12 @@
       <c r="G1459">
         <v>3</v>
       </c>
+      <c r="H1459">
+        <v>999</v>
+      </c>
+      <c r="I1459">
+        <v>999</v>
+      </c>
       <c r="J1459">
         <v>40000</v>
       </c>
@@ -72461,6 +73391,12 @@
       <c r="G1460">
         <v>3</v>
       </c>
+      <c r="H1460">
+        <v>999</v>
+      </c>
+      <c r="I1460">
+        <v>999</v>
+      </c>
       <c r="J1460">
         <v>35000</v>
       </c>
@@ -72505,6 +73441,12 @@
       <c r="G1461">
         <v>4</v>
       </c>
+      <c r="H1461">
+        <v>999</v>
+      </c>
+      <c r="I1461">
+        <v>999</v>
+      </c>
       <c r="J1461">
         <v>8680</v>
       </c>
@@ -72549,6 +73491,12 @@
       <c r="G1462">
         <v>3</v>
       </c>
+      <c r="H1462">
+        <v>999</v>
+      </c>
+      <c r="I1462">
+        <v>999</v>
+      </c>
       <c r="J1462">
         <v>50000</v>
       </c>
@@ -72593,6 +73541,12 @@
       <c r="G1463">
         <v>1</v>
       </c>
+      <c r="H1463">
+        <v>999</v>
+      </c>
+      <c r="I1463">
+        <v>999</v>
+      </c>
       <c r="J1463">
         <v>10000</v>
       </c>
@@ -72637,6 +73591,12 @@
       <c r="G1464">
         <v>3</v>
       </c>
+      <c r="H1464">
+        <v>999</v>
+      </c>
+      <c r="I1464">
+        <v>999</v>
+      </c>
       <c r="J1464">
         <v>30000</v>
       </c>
@@ -72681,6 +73641,12 @@
       <c r="G1465">
         <v>4</v>
       </c>
+      <c r="H1465">
+        <v>999</v>
+      </c>
+      <c r="I1465">
+        <v>999</v>
+      </c>
       <c r="J1465">
         <v>40000</v>
       </c>
@@ -72725,6 +73691,12 @@
       <c r="G1466">
         <v>1</v>
       </c>
+      <c r="H1466">
+        <v>999</v>
+      </c>
+      <c r="I1466">
+        <v>999</v>
+      </c>
       <c r="J1466">
         <v>7000</v>
       </c>
@@ -72769,6 +73741,12 @@
       <c r="G1467">
         <v>1</v>
       </c>
+      <c r="H1467">
+        <v>999</v>
+      </c>
+      <c r="I1467">
+        <v>999</v>
+      </c>
       <c r="J1467">
         <v>16000</v>
       </c>
@@ -72813,6 +73791,12 @@
       <c r="G1468">
         <v>3</v>
       </c>
+      <c r="H1468">
+        <v>999</v>
+      </c>
+      <c r="I1468">
+        <v>999</v>
+      </c>
       <c r="J1468">
         <v>10000</v>
       </c>
@@ -72857,6 +73841,12 @@
       <c r="G1469">
         <v>4</v>
       </c>
+      <c r="H1469">
+        <v>999</v>
+      </c>
+      <c r="I1469">
+        <v>999</v>
+      </c>
       <c r="J1469">
         <v>14000</v>
       </c>
@@ -72901,6 +73891,12 @@
       <c r="G1470">
         <v>4</v>
       </c>
+      <c r="H1470">
+        <v>999</v>
+      </c>
+      <c r="I1470">
+        <v>999</v>
+      </c>
       <c r="J1470">
         <v>150000</v>
       </c>
@@ -72945,6 +73941,12 @@
       <c r="G1471">
         <v>3</v>
       </c>
+      <c r="H1471">
+        <v>999</v>
+      </c>
+      <c r="I1471">
+        <v>999</v>
+      </c>
       <c r="J1471">
         <v>15000</v>
       </c>
@@ -72989,6 +73991,12 @@
       <c r="G1472">
         <v>4</v>
       </c>
+      <c r="H1472">
+        <v>999</v>
+      </c>
+      <c r="I1472">
+        <v>999</v>
+      </c>
       <c r="J1472">
         <v>12000</v>
       </c>
@@ -73033,6 +74041,12 @@
       <c r="G1473">
         <v>2</v>
       </c>
+      <c r="H1473">
+        <v>999</v>
+      </c>
+      <c r="I1473">
+        <v>999</v>
+      </c>
       <c r="J1473">
         <v>10000</v>
       </c>
@@ -73077,6 +74091,12 @@
       <c r="G1474">
         <v>4</v>
       </c>
+      <c r="H1474">
+        <v>999</v>
+      </c>
+      <c r="I1474">
+        <v>999</v>
+      </c>
       <c r="J1474">
         <v>20000</v>
       </c>
@@ -73121,6 +74141,12 @@
       <c r="G1475">
         <v>4</v>
       </c>
+      <c r="H1475">
+        <v>999</v>
+      </c>
+      <c r="I1475">
+        <v>999</v>
+      </c>
       <c r="J1475">
         <v>18000</v>
       </c>
@@ -73165,6 +74191,12 @@
       <c r="G1476">
         <v>4</v>
       </c>
+      <c r="H1476">
+        <v>999</v>
+      </c>
+      <c r="I1476">
+        <v>999</v>
+      </c>
       <c r="J1476">
         <v>42000</v>
       </c>
@@ -73209,6 +74241,12 @@
       <c r="G1477">
         <v>4</v>
       </c>
+      <c r="H1477">
+        <v>999</v>
+      </c>
+      <c r="I1477">
+        <v>999</v>
+      </c>
       <c r="J1477">
         <v>20000</v>
       </c>
@@ -73253,6 +74291,12 @@
       <c r="G1478">
         <v>4</v>
       </c>
+      <c r="H1478">
+        <v>999</v>
+      </c>
+      <c r="I1478">
+        <v>999</v>
+      </c>
       <c r="J1478">
         <v>35000</v>
       </c>
@@ -73297,6 +74341,12 @@
       <c r="G1479">
         <v>1</v>
       </c>
+      <c r="H1479">
+        <v>999</v>
+      </c>
+      <c r="I1479">
+        <v>999</v>
+      </c>
       <c r="J1479">
         <v>12000</v>
       </c>
@@ -73341,6 +74391,12 @@
       <c r="G1480">
         <v>3</v>
       </c>
+      <c r="H1480">
+        <v>999</v>
+      </c>
+      <c r="I1480">
+        <v>999</v>
+      </c>
       <c r="J1480">
         <v>10000</v>
       </c>
@@ -73385,6 +74441,12 @@
       <c r="G1481">
         <v>4</v>
       </c>
+      <c r="H1481">
+        <v>999</v>
+      </c>
+      <c r="I1481">
+        <v>999</v>
+      </c>
       <c r="J1481">
         <v>36000</v>
       </c>
@@ -73429,6 +74491,12 @@
       <c r="G1482">
         <v>4</v>
       </c>
+      <c r="H1482">
+        <v>999</v>
+      </c>
+      <c r="I1482">
+        <v>999</v>
+      </c>
       <c r="J1482">
         <v>19000</v>
       </c>
@@ -73473,6 +74541,12 @@
       <c r="G1483">
         <v>3</v>
       </c>
+      <c r="H1483">
+        <v>999</v>
+      </c>
+      <c r="I1483">
+        <v>999</v>
+      </c>
       <c r="J1483">
         <v>40000</v>
       </c>
@@ -73517,6 +74591,12 @@
       <c r="G1484">
         <v>4</v>
       </c>
+      <c r="H1484">
+        <v>999</v>
+      </c>
+      <c r="I1484">
+        <v>999</v>
+      </c>
       <c r="J1484">
         <v>30000</v>
       </c>
@@ -73561,6 +74641,12 @@
       <c r="G1485">
         <v>3</v>
       </c>
+      <c r="H1485">
+        <v>999</v>
+      </c>
+      <c r="I1485">
+        <v>999</v>
+      </c>
       <c r="J1485">
         <v>60000</v>
       </c>
@@ -73605,6 +74691,12 @@
       <c r="G1486">
         <v>3</v>
       </c>
+      <c r="H1486">
+        <v>999</v>
+      </c>
+      <c r="I1486">
+        <v>999</v>
+      </c>
       <c r="J1486">
         <v>6500</v>
       </c>
@@ -73649,6 +74741,12 @@
       <c r="G1487">
         <v>4</v>
       </c>
+      <c r="H1487">
+        <v>999</v>
+      </c>
+      <c r="I1487">
+        <v>999</v>
+      </c>
       <c r="J1487">
         <v>30000</v>
       </c>
@@ -73693,6 +74791,12 @@
       <c r="G1488">
         <v>3</v>
       </c>
+      <c r="H1488">
+        <v>999</v>
+      </c>
+      <c r="I1488">
+        <v>999</v>
+      </c>
       <c r="J1488">
         <v>60000</v>
       </c>
@@ -73737,6 +74841,12 @@
       <c r="G1489">
         <v>4</v>
       </c>
+      <c r="H1489">
+        <v>999</v>
+      </c>
+      <c r="I1489">
+        <v>999</v>
+      </c>
       <c r="J1489">
         <v>70000</v>
       </c>
@@ -73781,6 +74891,12 @@
       <c r="G1490">
         <v>4</v>
       </c>
+      <c r="H1490">
+        <v>999</v>
+      </c>
+      <c r="I1490">
+        <v>999</v>
+      </c>
       <c r="J1490">
         <v>45000</v>
       </c>
@@ -73825,6 +74941,12 @@
       <c r="G1491">
         <v>4</v>
       </c>
+      <c r="H1491">
+        <v>999</v>
+      </c>
+      <c r="I1491">
+        <v>999</v>
+      </c>
       <c r="J1491">
         <v>30000</v>
       </c>
@@ -73869,6 +74991,12 @@
       <c r="G1492">
         <v>3</v>
       </c>
+      <c r="H1492">
+        <v>999</v>
+      </c>
+      <c r="I1492">
+        <v>999</v>
+      </c>
       <c r="J1492">
         <v>20000</v>
       </c>
@@ -73913,6 +75041,12 @@
       <c r="G1493">
         <v>4</v>
       </c>
+      <c r="H1493">
+        <v>999</v>
+      </c>
+      <c r="I1493">
+        <v>999</v>
+      </c>
       <c r="J1493">
         <v>44000</v>
       </c>
@@ -73957,6 +75091,12 @@
       <c r="G1494">
         <v>3</v>
       </c>
+      <c r="H1494">
+        <v>999</v>
+      </c>
+      <c r="I1494">
+        <v>999</v>
+      </c>
       <c r="J1494">
         <v>20000</v>
       </c>
@@ -74001,6 +75141,12 @@
       <c r="G1495">
         <v>4</v>
       </c>
+      <c r="H1495">
+        <v>999</v>
+      </c>
+      <c r="I1495">
+        <v>999</v>
+      </c>
       <c r="J1495">
         <v>10000</v>
       </c>
@@ -74045,6 +75191,12 @@
       <c r="G1496">
         <v>4</v>
       </c>
+      <c r="H1496">
+        <v>999</v>
+      </c>
+      <c r="I1496">
+        <v>999</v>
+      </c>
       <c r="J1496">
         <v>9000</v>
       </c>
@@ -74089,6 +75241,12 @@
       <c r="G1497">
         <v>2</v>
       </c>
+      <c r="H1497">
+        <v>999</v>
+      </c>
+      <c r="I1497">
+        <v>999</v>
+      </c>
       <c r="J1497">
         <v>40000</v>
       </c>
@@ -74133,6 +75291,12 @@
       <c r="G1498">
         <v>3</v>
       </c>
+      <c r="H1498">
+        <v>999</v>
+      </c>
+      <c r="I1498">
+        <v>999</v>
+      </c>
       <c r="J1498">
         <v>18000</v>
       </c>
@@ -74177,6 +75341,12 @@
       <c r="G1499">
         <v>4</v>
       </c>
+      <c r="H1499">
+        <v>999</v>
+      </c>
+      <c r="I1499">
+        <v>999</v>
+      </c>
       <c r="J1499">
         <v>30000</v>
       </c>
@@ -74221,6 +75391,12 @@
       <c r="G1500">
         <v>1</v>
       </c>
+      <c r="H1500">
+        <v>999</v>
+      </c>
+      <c r="I1500">
+        <v>999</v>
+      </c>
       <c r="J1500">
         <v>9000</v>
       </c>
@@ -74265,6 +75441,12 @@
       <c r="G1501">
         <v>4</v>
       </c>
+      <c r="H1501">
+        <v>999</v>
+      </c>
+      <c r="I1501">
+        <v>999</v>
+      </c>
       <c r="J1501">
         <v>45000</v>
       </c>
@@ -74309,6 +75491,12 @@
       <c r="G1502">
         <v>3</v>
       </c>
+      <c r="H1502">
+        <v>999</v>
+      </c>
+      <c r="I1502">
+        <v>999</v>
+      </c>
       <c r="J1502">
         <v>10000</v>
       </c>
@@ -74353,6 +75541,12 @@
       <c r="G1503">
         <v>3</v>
       </c>
+      <c r="H1503">
+        <v>999</v>
+      </c>
+      <c r="I1503">
+        <v>999</v>
+      </c>
       <c r="J1503">
         <v>45000</v>
       </c>
@@ -74397,6 +75591,12 @@
       <c r="G1504">
         <v>3</v>
       </c>
+      <c r="H1504">
+        <v>999</v>
+      </c>
+      <c r="I1504">
+        <v>999</v>
+      </c>
       <c r="J1504">
         <v>40000</v>
       </c>
@@ -74441,6 +75641,12 @@
       <c r="G1505">
         <v>3</v>
       </c>
+      <c r="H1505">
+        <v>999</v>
+      </c>
+      <c r="I1505">
+        <v>999</v>
+      </c>
       <c r="J1505">
         <v>15000</v>
       </c>
@@ -74485,6 +75691,12 @@
       <c r="G1506">
         <v>1</v>
       </c>
+      <c r="H1506">
+        <v>999</v>
+      </c>
+      <c r="I1506">
+        <v>999</v>
+      </c>
       <c r="J1506">
         <v>14000</v>
       </c>
@@ -74529,6 +75741,12 @@
       <c r="G1507">
         <v>2</v>
       </c>
+      <c r="H1507">
+        <v>999</v>
+      </c>
+      <c r="I1507">
+        <v>999</v>
+      </c>
       <c r="J1507">
         <v>10000</v>
       </c>
@@ -74573,6 +75791,12 @@
       <c r="G1508">
         <v>1</v>
       </c>
+      <c r="H1508">
+        <v>999</v>
+      </c>
+      <c r="I1508">
+        <v>999</v>
+      </c>
       <c r="J1508">
         <v>12000</v>
       </c>
@@ -74617,6 +75841,12 @@
       <c r="G1509">
         <v>1</v>
       </c>
+      <c r="H1509">
+        <v>999</v>
+      </c>
+      <c r="I1509">
+        <v>999</v>
+      </c>
       <c r="J1509">
         <v>10000</v>
       </c>
@@ -74661,6 +75891,12 @@
       <c r="G1510">
         <v>3</v>
       </c>
+      <c r="H1510">
+        <v>999</v>
+      </c>
+      <c r="I1510">
+        <v>999</v>
+      </c>
       <c r="J1510">
         <v>12000</v>
       </c>
@@ -74705,6 +75941,12 @@
       <c r="G1511">
         <v>3</v>
       </c>
+      <c r="H1511">
+        <v>999</v>
+      </c>
+      <c r="I1511">
+        <v>999</v>
+      </c>
       <c r="J1511">
         <v>11000</v>
       </c>
@@ -74749,6 +75991,12 @@
       <c r="G1512">
         <v>3</v>
       </c>
+      <c r="H1512">
+        <v>999</v>
+      </c>
+      <c r="I1512">
+        <v>999</v>
+      </c>
       <c r="J1512">
         <v>12000</v>
       </c>
@@ -74793,6 +76041,12 @@
       <c r="G1513">
         <v>2</v>
       </c>
+      <c r="H1513">
+        <v>999</v>
+      </c>
+      <c r="I1513">
+        <v>999</v>
+      </c>
       <c r="J1513">
         <v>50000</v>
       </c>
@@ -74837,6 +76091,12 @@
       <c r="G1514">
         <v>2</v>
       </c>
+      <c r="H1514">
+        <v>999</v>
+      </c>
+      <c r="I1514">
+        <v>999</v>
+      </c>
       <c r="J1514">
         <v>5000</v>
       </c>
@@ -74881,6 +76141,12 @@
       <c r="G1515">
         <v>4</v>
       </c>
+      <c r="H1515">
+        <v>999</v>
+      </c>
+      <c r="I1515">
+        <v>999</v>
+      </c>
       <c r="J1515">
         <v>14000</v>
       </c>
@@ -74925,6 +76191,12 @@
       <c r="G1516">
         <v>1</v>
       </c>
+      <c r="H1516">
+        <v>999</v>
+      </c>
+      <c r="I1516">
+        <v>999</v>
+      </c>
       <c r="J1516">
         <v>2000</v>
       </c>
@@ -74969,6 +76241,12 @@
       <c r="G1517">
         <v>3</v>
       </c>
+      <c r="H1517">
+        <v>999</v>
+      </c>
+      <c r="I1517">
+        <v>999</v>
+      </c>
       <c r="J1517">
         <v>40000</v>
       </c>
@@ -75013,6 +76291,12 @@
       <c r="G1518">
         <v>1</v>
       </c>
+      <c r="H1518">
+        <v>999</v>
+      </c>
+      <c r="I1518">
+        <v>999</v>
+      </c>
       <c r="J1518">
         <v>8000</v>
       </c>
@@ -75057,6 +76341,12 @@
       <c r="G1519">
         <v>4</v>
       </c>
+      <c r="H1519">
+        <v>999</v>
+      </c>
+      <c r="I1519">
+        <v>999</v>
+      </c>
       <c r="J1519">
         <v>13000</v>
       </c>
@@ -75101,6 +76391,12 @@
       <c r="G1520">
         <v>3</v>
       </c>
+      <c r="H1520">
+        <v>999</v>
+      </c>
+      <c r="I1520">
+        <v>999</v>
+      </c>
       <c r="J1520">
         <v>10000</v>
       </c>
@@ -75145,6 +76441,12 @@
       <c r="G1521">
         <v>1</v>
       </c>
+      <c r="H1521">
+        <v>999</v>
+      </c>
+      <c r="I1521">
+        <v>999</v>
+      </c>
       <c r="J1521">
         <v>13000</v>
       </c>
@@ -75189,6 +76491,12 @@
       <c r="G1522">
         <v>3</v>
       </c>
+      <c r="H1522">
+        <v>999</v>
+      </c>
+      <c r="I1522">
+        <v>999</v>
+      </c>
       <c r="J1522">
         <v>9700</v>
       </c>
@@ -75233,6 +76541,12 @@
       <c r="G1523">
         <v>1</v>
       </c>
+      <c r="H1523">
+        <v>999</v>
+      </c>
+      <c r="I1523">
+        <v>999</v>
+      </c>
       <c r="J1523">
         <v>50000</v>
       </c>
@@ -75277,6 +76591,12 @@
       <c r="G1524">
         <v>1</v>
       </c>
+      <c r="H1524">
+        <v>999</v>
+      </c>
+      <c r="I1524">
+        <v>999</v>
+      </c>
       <c r="J1524">
         <v>30000</v>
       </c>
@@ -75321,6 +76641,12 @@
       <c r="G1525">
         <v>4</v>
       </c>
+      <c r="H1525">
+        <v>999</v>
+      </c>
+      <c r="I1525">
+        <v>999</v>
+      </c>
       <c r="J1525">
         <v>19000</v>
       </c>
@@ -75365,6 +76691,12 @@
       <c r="G1526">
         <v>1</v>
       </c>
+      <c r="H1526">
+        <v>999</v>
+      </c>
+      <c r="I1526">
+        <v>999</v>
+      </c>
       <c r="J1526">
         <v>8200</v>
       </c>
@@ -75409,6 +76741,12 @@
       <c r="G1527">
         <v>3</v>
       </c>
+      <c r="H1527">
+        <v>999</v>
+      </c>
+      <c r="I1527">
+        <v>999</v>
+      </c>
       <c r="J1527">
         <v>8000</v>
       </c>
@@ -75453,6 +76791,12 @@
       <c r="G1528">
         <v>3</v>
       </c>
+      <c r="H1528">
+        <v>999</v>
+      </c>
+      <c r="I1528">
+        <v>999</v>
+      </c>
       <c r="J1528">
         <v>8000</v>
       </c>
@@ -75497,6 +76841,12 @@
       <c r="G1529">
         <v>3</v>
       </c>
+      <c r="H1529">
+        <v>999</v>
+      </c>
+      <c r="I1529">
+        <v>999</v>
+      </c>
       <c r="J1529">
         <v>13000</v>
       </c>
@@ -75541,6 +76891,12 @@
       <c r="G1530">
         <v>4</v>
       </c>
+      <c r="H1530">
+        <v>999</v>
+      </c>
+      <c r="I1530">
+        <v>999</v>
+      </c>
       <c r="J1530">
         <v>25000</v>
       </c>
@@ -75585,6 +76941,12 @@
       <c r="G1531">
         <v>3</v>
       </c>
+      <c r="H1531">
+        <v>999</v>
+      </c>
+      <c r="I1531">
+        <v>999</v>
+      </c>
       <c r="J1531">
         <v>12600</v>
       </c>
@@ -75629,6 +76991,12 @@
       <c r="G1532">
         <v>4</v>
       </c>
+      <c r="H1532">
+        <v>999</v>
+      </c>
+      <c r="I1532">
+        <v>999</v>
+      </c>
       <c r="J1532">
         <v>15000</v>
       </c>
@@ -75673,6 +77041,12 @@
       <c r="G1533">
         <v>1</v>
       </c>
+      <c r="H1533">
+        <v>999</v>
+      </c>
+      <c r="I1533">
+        <v>999</v>
+      </c>
       <c r="J1533">
         <v>14000</v>
       </c>
@@ -75717,6 +77091,12 @@
       <c r="G1534">
         <v>4</v>
       </c>
+      <c r="H1534">
+        <v>999</v>
+      </c>
+      <c r="I1534">
+        <v>999</v>
+      </c>
       <c r="J1534">
         <v>35000</v>
       </c>
@@ -75761,6 +77141,12 @@
       <c r="G1535">
         <v>1</v>
       </c>
+      <c r="H1535">
+        <v>999</v>
+      </c>
+      <c r="I1535">
+        <v>999</v>
+      </c>
       <c r="J1535">
         <v>10000</v>
       </c>
@@ -75805,6 +77191,12 @@
       <c r="G1536">
         <v>4</v>
       </c>
+      <c r="H1536">
+        <v>999</v>
+      </c>
+      <c r="I1536">
+        <v>999</v>
+      </c>
       <c r="J1536">
         <v>15000</v>
       </c>
@@ -75849,6 +77241,12 @@
       <c r="G1537">
         <v>4</v>
       </c>
+      <c r="H1537">
+        <v>999</v>
+      </c>
+      <c r="I1537">
+        <v>999</v>
+      </c>
       <c r="J1537">
         <v>50000</v>
       </c>
@@ -75893,6 +77291,12 @@
       <c r="G1538">
         <v>2</v>
       </c>
+      <c r="H1538">
+        <v>999</v>
+      </c>
+      <c r="I1538">
+        <v>999</v>
+      </c>
       <c r="J1538">
         <v>11500</v>
       </c>
@@ -75937,6 +77341,12 @@
       <c r="G1539">
         <v>4</v>
       </c>
+      <c r="H1539">
+        <v>999</v>
+      </c>
+      <c r="I1539">
+        <v>999</v>
+      </c>
       <c r="J1539">
         <v>15000</v>
       </c>
@@ -75981,6 +77391,12 @@
       <c r="G1540">
         <v>4</v>
       </c>
+      <c r="H1540">
+        <v>999</v>
+      </c>
+      <c r="I1540">
+        <v>999</v>
+      </c>
       <c r="J1540">
         <v>9000</v>
       </c>
@@ -76025,6 +77441,12 @@
       <c r="G1541">
         <v>4</v>
       </c>
+      <c r="H1541">
+        <v>999</v>
+      </c>
+      <c r="I1541">
+        <v>999</v>
+      </c>
       <c r="J1541">
         <v>20000</v>
       </c>
@@ -76069,6 +77491,12 @@
       <c r="G1542">
         <v>3</v>
       </c>
+      <c r="H1542">
+        <v>999</v>
+      </c>
+      <c r="I1542">
+        <v>999</v>
+      </c>
       <c r="J1542">
         <v>9000</v>
       </c>
@@ -76113,6 +77541,12 @@
       <c r="G1543">
         <v>4</v>
       </c>
+      <c r="H1543">
+        <v>999</v>
+      </c>
+      <c r="I1543">
+        <v>999</v>
+      </c>
       <c r="J1543">
         <v>20000</v>
       </c>
@@ -76157,6 +77591,12 @@
       <c r="G1544">
         <v>4</v>
       </c>
+      <c r="H1544">
+        <v>999</v>
+      </c>
+      <c r="I1544">
+        <v>999</v>
+      </c>
       <c r="J1544">
         <v>40000</v>
       </c>
@@ -76201,6 +77641,12 @@
       <c r="G1545">
         <v>3</v>
       </c>
+      <c r="H1545">
+        <v>999</v>
+      </c>
+      <c r="I1545">
+        <v>999</v>
+      </c>
       <c r="J1545">
         <v>10000</v>
       </c>
@@ -76245,6 +77691,12 @@
       <c r="G1546">
         <v>3</v>
       </c>
+      <c r="H1546">
+        <v>999</v>
+      </c>
+      <c r="I1546">
+        <v>999</v>
+      </c>
       <c r="J1546">
         <v>15000</v>
       </c>
@@ -76289,6 +77741,12 @@
       <c r="G1547">
         <v>4</v>
       </c>
+      <c r="H1547">
+        <v>999</v>
+      </c>
+      <c r="I1547">
+        <v>999</v>
+      </c>
       <c r="J1547">
         <v>20000</v>
       </c>
@@ -76333,6 +77791,12 @@
       <c r="G1548">
         <v>4</v>
       </c>
+      <c r="H1548">
+        <v>999</v>
+      </c>
+      <c r="I1548">
+        <v>999</v>
+      </c>
       <c r="J1548">
         <v>12700</v>
       </c>
@@ -76377,6 +77841,12 @@
       <c r="G1549">
         <v>3</v>
       </c>
+      <c r="H1549">
+        <v>999</v>
+      </c>
+      <c r="I1549">
+        <v>999</v>
+      </c>
       <c r="J1549">
         <v>8000</v>
       </c>
@@ -76421,6 +77891,12 @@
       <c r="G1550">
         <v>3</v>
       </c>
+      <c r="H1550">
+        <v>999</v>
+      </c>
+      <c r="I1550">
+        <v>999</v>
+      </c>
       <c r="J1550">
         <v>30000</v>
       </c>
@@ -76465,6 +77941,12 @@
       <c r="G1551">
         <v>3</v>
       </c>
+      <c r="H1551">
+        <v>999</v>
+      </c>
+      <c r="I1551">
+        <v>999</v>
+      </c>
       <c r="J1551">
         <v>12000</v>
       </c>
@@ -76509,6 +77991,12 @@
       <c r="G1552">
         <v>3</v>
       </c>
+      <c r="H1552">
+        <v>999</v>
+      </c>
+      <c r="I1552">
+        <v>999</v>
+      </c>
       <c r="J1552">
         <v>8000</v>
       </c>
@@ -76553,6 +78041,12 @@
       <c r="G1553">
         <v>3</v>
       </c>
+      <c r="H1553">
+        <v>999</v>
+      </c>
+      <c r="I1553">
+        <v>999</v>
+      </c>
       <c r="J1553">
         <v>15000</v>
       </c>
@@ -76597,6 +78091,12 @@
       <c r="G1554">
         <v>3</v>
       </c>
+      <c r="H1554">
+        <v>999</v>
+      </c>
+      <c r="I1554">
+        <v>999</v>
+      </c>
       <c r="J1554">
         <v>10000</v>
       </c>
@@ -76641,6 +78141,12 @@
       <c r="G1555">
         <v>4</v>
       </c>
+      <c r="H1555">
+        <v>999</v>
+      </c>
+      <c r="I1555">
+        <v>999</v>
+      </c>
       <c r="J1555">
         <v>50000</v>
       </c>
@@ -76685,6 +78191,12 @@
       <c r="G1556">
         <v>3</v>
       </c>
+      <c r="H1556">
+        <v>999</v>
+      </c>
+      <c r="I1556">
+        <v>999</v>
+      </c>
       <c r="J1556">
         <v>4900</v>
       </c>
@@ -76729,6 +78241,12 @@
       <c r="G1557">
         <v>1</v>
       </c>
+      <c r="H1557">
+        <v>999</v>
+      </c>
+      <c r="I1557">
+        <v>999</v>
+      </c>
       <c r="J1557">
         <v>8000</v>
       </c>
@@ -76773,6 +78291,12 @@
       <c r="G1558">
         <v>3</v>
       </c>
+      <c r="H1558">
+        <v>999</v>
+      </c>
+      <c r="I1558">
+        <v>999</v>
+      </c>
       <c r="J1558">
         <v>30000</v>
       </c>
@@ -76817,6 +78341,12 @@
       <c r="G1559">
         <v>3</v>
       </c>
+      <c r="H1559">
+        <v>999</v>
+      </c>
+      <c r="I1559">
+        <v>999</v>
+      </c>
       <c r="J1559">
         <v>30000</v>
       </c>
@@ -76861,6 +78391,12 @@
       <c r="G1560">
         <v>3</v>
       </c>
+      <c r="H1560">
+        <v>999</v>
+      </c>
+      <c r="I1560">
+        <v>999</v>
+      </c>
       <c r="J1560">
         <v>20000</v>
       </c>
@@ -76905,6 +78441,12 @@
       <c r="G1561">
         <v>1</v>
       </c>
+      <c r="H1561">
+        <v>999</v>
+      </c>
+      <c r="I1561">
+        <v>999</v>
+      </c>
       <c r="J1561">
         <v>10500</v>
       </c>
@@ -76949,6 +78491,12 @@
       <c r="G1562">
         <v>4</v>
       </c>
+      <c r="H1562">
+        <v>999</v>
+      </c>
+      <c r="I1562">
+        <v>999</v>
+      </c>
       <c r="J1562">
         <v>90000</v>
       </c>
@@ -76993,6 +78541,12 @@
       <c r="G1563">
         <v>3</v>
       </c>
+      <c r="H1563">
+        <v>999</v>
+      </c>
+      <c r="I1563">
+        <v>999</v>
+      </c>
       <c r="J1563">
         <v>15000</v>
       </c>
@@ -77037,6 +78591,12 @@
       <c r="G1564">
         <v>3</v>
       </c>
+      <c r="H1564">
+        <v>999</v>
+      </c>
+      <c r="I1564">
+        <v>999</v>
+      </c>
       <c r="J1564">
         <v>21000</v>
       </c>
@@ -77081,6 +78641,12 @@
       <c r="G1565">
         <v>4</v>
       </c>
+      <c r="H1565">
+        <v>999</v>
+      </c>
+      <c r="I1565">
+        <v>999</v>
+      </c>
       <c r="J1565">
         <v>15000</v>
       </c>
@@ -77125,6 +78691,12 @@
       <c r="G1566">
         <v>3</v>
       </c>
+      <c r="H1566">
+        <v>999</v>
+      </c>
+      <c r="I1566">
+        <v>999</v>
+      </c>
       <c r="J1566">
         <v>10000</v>
       </c>
@@ -77169,6 +78741,12 @@
       <c r="G1567">
         <v>3</v>
       </c>
+      <c r="H1567">
+        <v>999</v>
+      </c>
+      <c r="I1567">
+        <v>999</v>
+      </c>
       <c r="J1567">
         <v>30000</v>
       </c>
@@ -77213,6 +78791,12 @@
       <c r="G1568">
         <v>3</v>
       </c>
+      <c r="H1568">
+        <v>999</v>
+      </c>
+      <c r="I1568">
+        <v>999</v>
+      </c>
       <c r="J1568">
         <v>27000</v>
       </c>
@@ -77257,6 +78841,12 @@
       <c r="G1569">
         <v>3</v>
       </c>
+      <c r="H1569">
+        <v>999</v>
+      </c>
+      <c r="I1569">
+        <v>999</v>
+      </c>
       <c r="J1569">
         <v>35000</v>
       </c>
@@ -77301,6 +78891,12 @@
       <c r="G1570">
         <v>3</v>
       </c>
+      <c r="H1570">
+        <v>999</v>
+      </c>
+      <c r="I1570">
+        <v>999</v>
+      </c>
       <c r="J1570">
         <v>13000</v>
       </c>
@@ -77344,6 +78940,12 @@
       </c>
       <c r="G1571">
         <v>4</v>
+      </c>
+      <c r="H1571">
+        <v>999</v>
+      </c>
+      <c r="I1571">
+        <v>999</v>
       </c>
       <c r="J1571">
         <v>20000</v>

</xml_diff>